<commit_message>
add fomc cycle odd/even week dummies draft
</commit_message>
<xml_diff>
--- a/data/FOMC_Cycle_dates_2018_mar2023.xlsx
+++ b/data/FOMC_Cycle_dates_2018_mar2023.xlsx
@@ -5,16 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felixreichel/Documents/UNI/WIWI_Bachelor/2023S/Bachelorarbeit/Git/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felixreichel/Documents/UNI/WIWI_Bachelor/2023S/SE Bachelorarbeit/Git/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3660" yWindow="-16980" windowWidth="28800" windowHeight="17300" tabRatio="500"/>
+    <workbookView xWindow="1300" yWindow="-19900" windowWidth="28800" windowHeight="17300" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -412,8 +412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="99" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -457,7 +457,6 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
-        <f>DATE(2023,3,21)</f>
         <v>45006</v>
       </c>
       <c r="B11" s="4">
@@ -720,7 +719,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="4">
-        <v>37318</v>
+        <v>43893</v>
       </c>
       <c r="B40" s="4">
         <v>37318</v>

</xml_diff>